<commit_message>
Update notes on About tab of ccs/CC to discuss energy input data (#59)
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A6DB72-71D0-45E8-A676-F28304F79379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="13860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,22 @@
     <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId5"/>
     <sheet name="CC-EUpTCS" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
   <si>
     <t>Source:</t>
   </si>
@@ -251,13 +262,31 @@
     <t>carbon capture and sequestration, for both the power and industry</t>
   </si>
   <si>
-    <t>sectors.</t>
+    <t>sectors.  It also includes data on energy use per ton CO2 sequestered.</t>
+  </si>
+  <si>
+    <t>The energy use value here should exclude any energy that is not additional</t>
+  </si>
+  <si>
+    <t>to the energy already accounted for in indst/BIFUbC or the heat rates in the</t>
+  </si>
+  <si>
+    <t>electricity sector.  For example, if a steel mill has excess process heat that</t>
+  </si>
+  <si>
+    <t>isn't being used, and they use it to power CCS, that heat should be excluded</t>
+  </si>
+  <si>
+    <t>from here, since it does not increase the overall energy demand of the steel</t>
+  </si>
+  <si>
+    <t>mill.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -544,6 +573,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -579,6 +625,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,12 +817,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -834,68 +895,101 @@
       <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -903,7 +997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1676,7 +1770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1892,7 +1986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1937,7 +2031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1982,7 +2076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>

</xml_diff>

<commit_message>
Updates fixing methodological error in CCS capital cost calculations
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A6DB72-71D0-45E8-A676-F28304F79379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686D6B6B-9F94-4EBA-B7C8-9C6029A245C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t>Source:</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t>$/(kg/h)</t>
-  </si>
-  <si>
     <t>Cycle</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Electricity (IGCC)</t>
   </si>
   <si>
-    <t>Operating hrs/yr</t>
-  </si>
-  <si>
     <t>kg/ton</t>
   </si>
   <si>
@@ -281,6 +275,42 @@
   </si>
   <si>
     <t>mill.</t>
+  </si>
+  <si>
+    <t>Capacity Factor</t>
+  </si>
+  <si>
+    <t>Capture Capital Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Reference Emissions Rate (kg/kWh)</t>
+  </si>
+  <si>
+    <t>Capture Emissions Rate (kg/kWh)</t>
+  </si>
+  <si>
+    <t>Capture Amount (kg/kWh)</t>
+  </si>
+  <si>
+    <t>1 kW plant</t>
+  </si>
+  <si>
+    <t>Capital Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Electricity (PC)</t>
+  </si>
+  <si>
+    <t>Reference Emissions Rate (kg CO2/kWh)</t>
+  </si>
+  <si>
+    <t>Capture Emissions Rate (kg CO2/kWh)</t>
+  </si>
+  <si>
+    <t>Capture Rate (kg CO2/kWh)</t>
+  </si>
+  <si>
+    <t>Annual Capture (tons CO2/kW)</t>
   </si>
 </sst>
 </file>
@@ -438,7 +468,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -478,6 +508,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -820,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -830,17 +861,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +884,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -873,22 +904,22 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,32 +927,32 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -929,62 +960,62 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -998,9 +1029,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1008,40 +1041,41 @@
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="10">
         <v>2000</v>
@@ -1078,7 +1112,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="16">
         <v>1401</v>
@@ -1101,7 +1135,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="16">
         <v>7.9</v>
@@ -1124,7 +1158,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="16">
         <v>8081</v>
@@ -1147,7 +1181,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="16">
         <v>305</v>
@@ -1170,7 +1204,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="16">
         <v>2.65</v>
@@ -1193,7 +1227,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="16">
         <v>0.19400000000000001</v>
@@ -1216,7 +1250,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -1227,7 +1261,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="16">
         <v>6570</v>
@@ -1250,7 +1284,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="16">
         <v>15</v>
@@ -1273,7 +1307,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="16">
         <v>1.24</v>
@@ -1296,7 +1330,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="16">
         <v>90</v>
@@ -1317,9 +1351,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1328,9 +1362,9 @@
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="16">
         <v>0.752</v>
@@ -1351,9 +1385,9 @@
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="16">
         <v>32</v>
@@ -1373,10 +1407,13 @@
       <c r="G19" s="17">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="16">
         <v>10</v>
@@ -1396,10 +1433,17 @@
       <c r="G20" s="17">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f>E27</f>
+        <v>1718</v>
+      </c>
+      <c r="M20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="16">
         <v>7.9</v>
@@ -1419,10 +1463,17 @@
       <c r="G21" s="17">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f>E18</f>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="M21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="16">
         <v>4.99</v>
@@ -1442,10 +1493,17 @@
       <c r="G22" s="17">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f>E28</f>
+        <v>0.09</v>
+      </c>
+      <c r="M22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="16">
         <v>42.2</v>
@@ -1465,10 +1523,17 @@
       <c r="G23" s="17">
         <v>60.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f>L21-L22</f>
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="M23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1476,10 +1541,14 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f>L20/L23</f>
+        <v>2541.4201183431951</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="16">
         <v>85.4</v>
@@ -1500,9 +1569,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="16">
         <v>9462</v>
@@ -1523,9 +1592,9 @@
         <v>6308</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="16">
         <v>1909</v>
@@ -1546,9 +1615,9 @@
         <v>894</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="16">
         <v>8.7999999999999995E-2</v>
@@ -1569,9 +1638,9 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="16">
         <v>43.6</v>
@@ -1592,9 +1661,9 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="16">
         <v>11.7</v>
@@ -1615,9 +1684,9 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="16">
         <v>11.6</v>
@@ -1638,9 +1707,9 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="16">
         <v>6.69</v>
@@ -1663,7 +1732,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="16">
         <v>36.1</v>
@@ -1686,7 +1755,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1697,7 +1766,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="16">
         <v>1.7</v>
@@ -1720,7 +1789,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="16">
         <v>14.6</v>
@@ -1743,7 +1812,7 @@
     </row>
     <row r="37" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="21">
         <v>26</v>
@@ -1771,20 +1840,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1792,191 +1863,227 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="B3">
-        <f>'Table 2'!C9</f>
-        <v>275</v>
+        <f>'Table 2'!E27</f>
+        <v>1718</v>
       </c>
       <c r="C3">
-        <f>'Table 2'!G9</f>
-        <v>829</v>
+        <f>'Table 2'!G27</f>
+        <v>894</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B4">
-        <f>'Table 2'!C13</f>
+        <f>'Table 2'!E18</f>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="C4">
+        <f>'Table 2'!G18</f>
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <f>'Table 2'!E28</f>
+        <v>0.09</v>
+      </c>
+      <c r="C5">
+        <f>'Table 2'!G28</f>
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <f>B4-B5</f>
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="C6">
+        <f>C4-C5</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <f>'Table 2'!E13</f>
         <v>6570</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <f>'Table 2'!G13</f>
         <v>6570</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="31">
+        <f>B6*B7/1000</f>
+        <v>4.441320000000001</v>
+      </c>
+      <c r="C8" s="31">
+        <f>C6*C7/1000</f>
+        <v>1.9710000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="23">
+        <f>B3/B8</f>
+        <v>386.821935820882</v>
+      </c>
+      <c r="C9" s="23">
+        <f>C3/C8</f>
+        <v>453.57686453576855</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="23">
-        <f>B3/B4*B5</f>
-        <v>41.856925418569254</v>
-      </c>
-      <c r="C6" s="23">
-        <f>C3/C4*C5</f>
-        <v>126.17960426179603</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
         <f>'Table 2'!C10</f>
         <v>2.39</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <f>'Table 2'!G10</f>
         <v>4.68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
         <v>1E-3</v>
       </c>
-      <c r="C12">
+      <c r="C15">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
         <v>1000</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="26">
-        <f>B11*B12*B13</f>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="26">
+        <f>B14*B15*B16</f>
         <v>2.39</v>
       </c>
-      <c r="C14" s="26">
-        <f>C11*C12*C13</f>
+      <c r="C17" s="26">
+        <f>C14*C15*C16</f>
         <v>4.68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19">
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
         <f>'Table 2'!C11</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <f>'Table 2'!G11</f>
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
         <v>1000</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24">
         <v>3412</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>3412</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22">
-        <f>B19*B20*B21</f>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25">
+        <f>B22*B23*B24</f>
         <v>460620</v>
       </c>
-      <c r="C22">
-        <f>C19*C20*C21</f>
+      <c r="C25">
+        <f>C22*C23*C24</f>
         <v>1013364</v>
       </c>
     </row>
@@ -1992,8 +2099,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,25 +2111,25 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="28">
-        <f>Calculations!B6</f>
-        <v>41.856925418569254</v>
+        <f>Calculations!B9</f>
+        <v>386.821935820882</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="28">
-        <f>Calculations!C6</f>
-        <v>126.17960426179603</v>
+        <f>Calculations!C9</f>
+        <v>453.57686453576855</v>
       </c>
     </row>
   </sheetData>
@@ -2049,24 +2156,24 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2">
-        <f>Calculations!B14</f>
+        <f>Calculations!B17</f>
         <v>2.39</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3">
-        <f>Calculations!C14</f>
+        <f>Calculations!C17</f>
         <v>4.68</v>
       </c>
     </row>
@@ -2094,24 +2201,24 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2">
-        <f>Calculations!B22</f>
+        <f>Calculations!B25</f>
         <v>460620</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3">
-        <f>Calculations!C22</f>
+        <f>Calculations!C25</f>
         <v>1013364</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to CCS input calculations.
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686D6B6B-9F94-4EBA-B7C8-9C6029A245C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CEF36D-133E-40BD-AB2E-5078AB52F720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>Source:</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>Industry (NGCC)</t>
-  </si>
-  <si>
-    <t>Electricity (IGCC)</t>
   </si>
   <si>
     <t>kg/ton</t>
@@ -861,17 +858,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,7 +881,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,22 +901,22 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,32 +924,32 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,12 +962,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1000,22 +997,22 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="L19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1438,7 +1435,7 @@
         <v>1718</v>
       </c>
       <c r="M20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1468,7 +1465,7 @@
         <v>0.76600000000000001</v>
       </c>
       <c r="M21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1498,7 +1495,7 @@
         <v>0.09</v>
       </c>
       <c r="M22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1528,7 +1525,7 @@
         <v>0.67600000000000005</v>
       </c>
       <c r="M23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1842,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1852,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1863,7 +1860,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>44</v>
@@ -1871,7 +1868,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <f>'Table 2'!E27</f>
@@ -1884,7 +1881,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <f>'Table 2'!E18</f>
@@ -1897,7 +1894,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <f>'Table 2'!E28</f>
@@ -1910,7 +1907,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <f>B4-B5</f>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7">
         <f>'Table 2'!E13</f>
@@ -1936,7 +1933,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="31">
         <f>B6*B7/1000</f>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="23">
         <f>B3/B8</f>
@@ -1962,7 +1959,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1970,7 +1967,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
@@ -1981,8 +1978,8 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f>'Table 2'!C10</f>
-        <v>2.39</v>
+        <f>'Table 2'!E10</f>
+        <v>5</v>
       </c>
       <c r="C14">
         <f>'Table 2'!G10</f>
@@ -1991,7 +1988,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>1E-3</v>
@@ -2002,7 +1999,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>1000</v>
@@ -2013,11 +2010,11 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="26">
         <f>B14*B15*B16</f>
-        <v>2.39</v>
+        <v>5</v>
       </c>
       <c r="C17" s="26">
         <f>C14*C15*C16</f>
@@ -2026,14 +2023,14 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>44</v>
@@ -2044,8 +2041,8 @@
         <v>11</v>
       </c>
       <c r="B22">
-        <f>'Table 2'!C11</f>
-        <v>0.13500000000000001</v>
+        <f>'Table 2'!E11</f>
+        <v>0.19600000000000001</v>
       </c>
       <c r="C22">
         <f>'Table 2'!G11</f>
@@ -2054,7 +2051,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>1000</v>
@@ -2065,7 +2062,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>3412</v>
@@ -2076,11 +2073,11 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <f>B22*B23*B24</f>
-        <v>460620</v>
+        <v>668752</v>
       </c>
       <c r="C25">
         <f>C22*C23*C24</f>
@@ -2099,7 +2096,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2111,12 +2108,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="28">
         <f>Calculations!B9</f>
@@ -2125,7 +2122,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="28">
         <f>Calculations!C9</f>
@@ -2145,7 +2142,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,21 +2153,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <f>Calculations!B17</f>
-        <v>2.39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <f>Calculations!C17</f>
@@ -2201,21 +2198,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <f>Calculations!B25</f>
-        <v>460620</v>
+        <v>668752</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <f>Calculations!C25</f>

</xml_diff>

<commit_message>
Updates to CCS capital costs
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CEF36D-133E-40BD-AB2E-5078AB52F720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C475A7-5B31-48E3-97C8-09CE78BDD5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,9 +292,6 @@
     <t>1 kW plant</t>
   </si>
   <si>
-    <t>Capital Cost ($/kW)</t>
-  </si>
-  <si>
     <t>Electricity (PC)</t>
   </si>
   <si>
@@ -308,15 +305,19 @@
   </si>
   <si>
     <t>Annual Capture (tons CO2/kW)</t>
+  </si>
+  <si>
+    <t>Incremental Capital Cost ($/kW)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -465,7 +466,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -506,6 +507,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1029,7 +1031,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="I24" sqref="I24:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1842,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B25"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1862,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>44</v>
@@ -1868,20 +1870,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B3">
-        <f>'Table 2'!E27</f>
-        <v>1718</v>
+        <f>'Table 2'!E27-'Table 2'!E6</f>
+        <v>623</v>
       </c>
       <c r="C3">
-        <f>'Table 2'!G27</f>
-        <v>894</v>
+        <f>'Table 2'!G27-'Table 2'!G6</f>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <f>'Table 2'!E18</f>
@@ -1894,7 +1896,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <f>'Table 2'!E28</f>
@@ -1907,7 +1909,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <f>B4-B5</f>
@@ -1933,7 +1935,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="31">
         <f>B6*B7/1000</f>
@@ -1950,11 +1952,11 @@
       </c>
       <c r="B9" s="23">
         <f>B3/B8</f>
-        <v>386.821935820882</v>
+        <v>140.27361234948165</v>
       </c>
       <c r="C9" s="23">
         <f>C3/C8</f>
-        <v>453.57686453576855</v>
+        <v>187.21461187214609</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1967,7 +1969,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
@@ -2030,7 +2032,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>44</v>
@@ -2097,7 +2099,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2119,7 @@
       </c>
       <c r="B2" s="28">
         <f>Calculations!B9</f>
-        <v>386.821935820882</v>
+        <v>140.27361234948165</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
@@ -2126,7 +2128,7 @@
       </c>
       <c r="B3" s="28">
         <f>Calculations!C9</f>
-        <v>453.57686453576855</v>
+        <v>187.21461187214609</v>
       </c>
     </row>
   </sheetData>
@@ -2142,7 +2144,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B40"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2162,7 @@
       <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="32">
         <f>Calculations!B17</f>
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Same updates as previous commit
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C475A7-5B31-48E3-97C8-09CE78BDD5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C6C654-6F51-4D06-876F-005809EAC53B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,35 @@
     <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId5"/>
     <sheet name="CC-EUpTCS" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$41</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">About!$A$39</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0.15</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
   <si>
     <t>Source:</t>
   </si>
@@ -277,21 +306,6 @@
     <t>Capacity Factor</t>
   </si>
   <si>
-    <t>Capture Capital Cost ($/kW)</t>
-  </si>
-  <si>
-    <t>Reference Emissions Rate (kg/kWh)</t>
-  </si>
-  <si>
-    <t>Capture Emissions Rate (kg/kWh)</t>
-  </si>
-  <si>
-    <t>Capture Amount (kg/kWh)</t>
-  </si>
-  <si>
-    <t>1 kW plant</t>
-  </si>
-  <si>
     <t>Electricity (PC)</t>
   </si>
   <si>
@@ -308,6 +322,15 @@
   </si>
   <si>
     <t>Incremental Capital Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Capital Recovery Factor</t>
+  </si>
+  <si>
+    <t>Lifetime (assumption)</t>
+  </si>
+  <si>
+    <t>Interest Rate (calculated)</t>
   </si>
 </sst>
 </file>
@@ -461,12 +484,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -508,11 +532,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -848,12 +875,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
@@ -997,24 +1027,49 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <f>(A41*(1+A41)^A40)/(((1+A41)^A40)-1)</f>
+        <v>0.14999998661846878</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
+        <v>0.14758719147187924</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1028,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:J29"/>
+      <selection activeCell="P27" sqref="K16:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1405,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -1361,7 +1416,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
@@ -1384,7 +1439,7 @@
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
@@ -1406,11 +1461,8 @@
       <c r="G19" s="17">
         <v>12</v>
       </c>
-      <c r="L19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
@@ -1432,15 +1484,8 @@
       <c r="G20" s="17">
         <v>16.600000000000001</v>
       </c>
-      <c r="L20">
-        <f>E27</f>
-        <v>1718</v>
-      </c>
-      <c r="M20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
@@ -1462,15 +1507,8 @@
       <c r="G21" s="17">
         <v>2.4</v>
       </c>
-      <c r="L21">
-        <f>E18</f>
-        <v>0.76600000000000001</v>
-      </c>
-      <c r="M21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>29</v>
       </c>
@@ -1492,15 +1530,8 @@
       <c r="G22" s="17">
         <v>3.1</v>
       </c>
-      <c r="L22">
-        <f>E28</f>
-        <v>0.09</v>
-      </c>
-      <c r="M22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>30</v>
       </c>
@@ -1522,15 +1553,8 @@
       <c r="G23" s="17">
         <v>60.1</v>
       </c>
-      <c r="L23">
-        <f>L21-L22</f>
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="M23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>31</v>
       </c>
@@ -1540,12 +1564,8 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
-      <c r="L24">
-        <f>L20/L23</f>
-        <v>2541.4201183431951</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1588,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
@@ -1591,7 +1611,7 @@
         <v>6308</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1634,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>25</v>
       </c>
@@ -1637,7 +1657,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>26</v>
       </c>
@@ -1660,7 +1680,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>27</v>
       </c>
@@ -1683,7 +1703,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>28</v>
       </c>
@@ -1706,7 +1726,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>29</v>
       </c>
@@ -1842,7 +1862,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1882,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>44</v>
@@ -1870,7 +1890,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <f>'Table 2'!E27-'Table 2'!E6</f>
@@ -1883,7 +1903,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <f>'Table 2'!E18</f>
@@ -1896,7 +1916,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <f>'Table 2'!E28</f>
@@ -1909,7 +1929,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <f>B4-B5</f>
@@ -1935,7 +1955,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B8" s="31">
         <f>B6*B7/1000</f>
@@ -1951,12 +1971,12 @@
         <v>46</v>
       </c>
       <c r="B9" s="23">
-        <f>B3/B8</f>
-        <v>140.27361234948165</v>
+        <f>B3/B8*About!$A$39*30</f>
+        <v>631.23119926039578</v>
       </c>
       <c r="C9" s="23">
-        <f>C3/C8</f>
-        <v>187.21461187214609</v>
+        <f>C3/C8*About!$A$39*30</f>
+        <v>842.46567826811213</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1969,7 +1989,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
@@ -2032,7 +2052,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>44</v>
@@ -2119,7 +2139,7 @@
       </c>
       <c r="B2" s="28">
         <f>Calculations!B9</f>
-        <v>140.27361234948165</v>
+        <v>631.23119926039578</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
@@ -2128,7 +2148,7 @@
       </c>
       <c r="B3" s="28">
         <f>Calculations!C9</f>
-        <v>187.21461187214609</v>
+        <v>842.46567826811213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit CCS data and add smoothing time for CCS capital costs
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A143292D-6B98-4E21-8DC8-B7F504BB10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC8057-3D10-459B-A73B-36B6485E5AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="98">
   <si>
     <t>Source:</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Energy Use per Ton Sequestered (BTU/gram CO2e)</t>
+  </si>
+  <si>
+    <t>*We use ethanol production as a proxy for the chemicals industry, as we expect ammonia production to be decarbonized via</t>
+  </si>
+  <si>
+    <t>hydrogen electrolysis in our BAU case.</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -900,8 +906,8 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,15 +957,15 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A2,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A2,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -988,15 +994,15 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A3,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A3,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1025,15 +1031,15 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A4,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A4,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1062,15 +1068,15 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A5,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A5,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1099,15 +1105,15 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A6,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A6,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1136,15 +1142,15 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A7,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A7,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1173,15 +1179,15 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A8,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A8,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1210,15 +1216,15 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A9,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A9,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1247,15 +1253,16 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>B9</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C10">
+        <f t="shared" ref="C10:D10" si="0">C9</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f t="shared" si="0"/>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1284,15 +1291,15 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A11,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>3.6323360324901186E-7</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A11,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1321,15 +1328,15 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A12,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A12,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1358,15 +1365,15 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A13,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A13,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1395,15 +1402,15 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A14,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A14,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.7187140690415008E-6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1432,15 +1439,15 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A15,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A15,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.7187140690415008E-6</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1469,15 +1476,15 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A16,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A16,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1506,15 +1513,15 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A17,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A17,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1543,15 +1550,15 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A18,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A18,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1580,15 +1587,15 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A19,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A19,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1617,15 +1624,15 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A20,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A20,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1654,15 +1661,15 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A21,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A21,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1691,15 +1698,15 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A22,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A22,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1728,15 +1735,15 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A23,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A23,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1765,15 +1772,15 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A24,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>3.0269466937417661E-7</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A24,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1802,15 +1809,15 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A25,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A25,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1839,15 +1846,15 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A26,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.8431147099868251E-7</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A26,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.8700614037285907E-6</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1883,7 +1890,7 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1912,7 +1919,7 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <f>Data!E24/10^12</f>
+        <f>Data!E25/10^12</f>
         <v>6.1418537999999999E-7</v>
       </c>
     </row>
@@ -1929,7 +1936,7 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <f>Data!E25/10^12</f>
+        <f>Data!E26/10^12</f>
         <v>8.7009595499999985E-6</v>
       </c>
     </row>
@@ -1997,10 +2004,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA25B772-A559-4F07-971A-AC3B6FFE9BE6}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2479,185 +2486,213 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B22" t="str">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B23" t="str">
         <f>B3</f>
         <v>Natural Gas Processing</v>
       </c>
-      <c r="C22" t="str">
-        <f t="shared" ref="C22:I22" si="7">C3</f>
+      <c r="C23" t="str">
+        <f t="shared" ref="C23:I23" si="7">C3</f>
         <v>Ethanol Production</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D23" t="str">
         <f t="shared" si="7"/>
         <v>Ammonia Production</v>
       </c>
-      <c r="E22" t="str">
+      <c r="E23" t="str">
         <f t="shared" si="7"/>
         <v>Hydrogen Production</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F23" t="str">
         <f t="shared" si="7"/>
         <v>Cement Plant</v>
       </c>
-      <c r="G22" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="7"/>
         <v>Refinery Fluidized Catalytic Converter</v>
       </c>
-      <c r="H22" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="7"/>
         <v>Iron and Steel Plant</v>
       </c>
-      <c r="I22" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="7"/>
         <v>Industrial Furnace</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f>AVERAGE(B5,B15)*10^6/B14*(1+B19)</f>
         <v>96.37385234743823</v>
       </c>
-      <c r="C23">
-        <f t="shared" ref="C23:I23" si="8">AVERAGE(C5,C15)*10^6/C14*(1+C19)</f>
+      <c r="C24">
+        <f t="shared" ref="C24:I24" si="8">AVERAGE(C5,C15)*10^6/C14*(1+C19)</f>
         <v>90.318959616700909</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <f t="shared" si="8"/>
         <v>86.245524017467261</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <f t="shared" si="8"/>
         <v>237.598625</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <f t="shared" si="8"/>
         <v>241.26666666666668</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <f t="shared" si="8"/>
         <v>498.34125</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <f t="shared" si="8"/>
         <v>177.6637793116993</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <f t="shared" si="8"/>
         <v>571.58457392593505</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>AVERAGE(B6,B16)*About!$A$30</f>
         <v>341214.10000000003</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>AVERAGE(C6,C16)*About!$A$30</f>
         <v>409456.92</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f>AVERAGE(D6,D16)*About!$A$30</f>
         <v>341214.10000000003</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f>AVERAGE(E6,E16)*About!$A$30</f>
         <v>614185.38</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <f>AVERAGE(F6,F16)*About!$A$30</f>
         <v>545942.56000000006</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <f>AVERAGE(G6,G16)*About!$A$30</f>
         <v>477699.74000000005</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <f>AVERAGE(H6,H16)*About!$A$30</f>
         <v>545942.56000000006</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <f>AVERAGE(I6,I16)*About!$A$30</f>
         <v>545942.56000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <f>AVERAGE(B7,B17)*About!$A$30</f>
         <v>0</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>AVERAGE(C7,C17)*About!$A$30</f>
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f>AVERAGE(D7,D17)*About!$A$30</f>
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f>AVERAGE(E7,E17)*About!$A$30</f>
         <v>8700959.5499999989</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <f>AVERAGE(F7,F17)*About!$A$30</f>
         <v>8700959.5499999989</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <f>AVERAGE(G7,G17)*About!$A$30</f>
         <v>8700959.5499999989</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <f>AVERAGE(H7,H17)*About!$A$30</f>
         <v>8700959.5499999989</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <f>AVERAGE(I7,I17)*About!$A$30</f>
         <v>8871566.5999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B26">
-        <f>AVERAGE(B8,B18)*B23</f>
+      <c r="B27">
+        <f>AVERAGE(B8,B18)*B24</f>
         <v>5.7824311408462936</v>
       </c>
-      <c r="C26">
-        <f t="shared" ref="C26:I26" si="9">AVERAGE(C8,C18)*C23</f>
+      <c r="C27">
+        <f t="shared" ref="C27:I27" si="9">AVERAGE(C8,C18)*C24</f>
         <v>6.3223271731690645</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f t="shared" si="9"/>
         <v>4.3122762008733631</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <f t="shared" si="9"/>
         <v>11.87993125</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <f t="shared" si="9"/>
         <v>16.888666666666669</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <f t="shared" si="9"/>
         <v>19.93365</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <f t="shared" si="9"/>
         <v>8.8831889655849654</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <f t="shared" si="9"/>
         <v>22.863382957037402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2708,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2692,7 +2727,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2701,7 +2736,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2710,7 +2745,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2719,7 +2754,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2728,7 +2763,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2737,7 +2772,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2746,7 +2781,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2755,7 +2790,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2764,8 +2799,8 @@
         <v>17</v>
       </c>
       <c r="B10" s="3">
-        <f>Data!$I$23*About!$A$28</f>
-        <v>507.0587751909739</v>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A10,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
+        <v>442.08384092059458</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2773,7 +2808,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2782,7 +2817,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2791,7 +2826,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2800,7 +2835,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2809,7 +2844,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2818,7 +2853,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2827,7 +2862,7 @@
         <v>24</v>
       </c>
       <c r="B17" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2836,7 +2871,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2845,7 +2880,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2854,7 +2889,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2863,7 +2898,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2872,7 +2907,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2881,7 +2916,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2890,7 +2925,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2899,7 +2934,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2908,7 +2943,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2925,7 +2960,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2944,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A2,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2953,7 +2988,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A3,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2962,7 +2997,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A4,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2971,7 +3006,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A5,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2980,7 +3015,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A6,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2989,7 +3024,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A7,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -2998,7 +3033,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A8,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3007,7 +3042,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A9,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3016,7 +3051,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>Data!$I$24*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3025,8 +3060,8 @@
         <v>18</v>
       </c>
       <c r="B11" s="3">
-        <f>Data!$I$23*About!$A$28</f>
-        <v>507.0587751909739</v>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A11,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
+        <v>80.122912914199276</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3034,7 +3069,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A12,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3043,7 +3078,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A13,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3052,8 +3087,8 @@
         <v>21</v>
       </c>
       <c r="B14" s="3">
-        <f>Data!$I$23*About!$A$28</f>
-        <v>507.0587751909739</v>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A14,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
+        <v>214.0302346757544</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3061,8 +3096,8 @@
         <v>22</v>
       </c>
       <c r="B15" s="3">
-        <f>Data!$I$23*About!$A$28</f>
-        <v>507.0587751909739</v>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A15,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
+        <v>157.60743456534033</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3070,7 +3105,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A16,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3079,7 +3114,7 @@
         <v>24</v>
       </c>
       <c r="B17" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A17,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3088,7 +3123,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A18,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3097,7 +3132,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A19,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3106,7 +3141,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A20,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3115,7 +3150,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A21,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3124,7 +3159,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A22,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3133,7 +3168,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A23,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3142,8 +3177,8 @@
         <v>31</v>
       </c>
       <c r="B24" s="3">
-        <f>Data!$I$23*About!$A$28</f>
-        <v>507.0587751909739</v>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A24,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
+        <v>85.494272870387022</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -3151,7 +3186,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A25,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3160,7 +3195,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="3">
-        <f>Data!$I$23*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$24:$24,MATCH('CC-CCoIPCE'!A26,Data!$22:$22,0)),Data!$I$24)*About!$A$28</f>
         <v>507.0587751909739</v>
       </c>
     </row>
@@ -3196,7 +3231,7 @@
         <v>79</v>
       </c>
       <c r="B2" s="3">
-        <f>Data!E23*About!$A$28</f>
+        <f>Data!E24*About!$A$28</f>
         <v>210.77627576977025</v>
       </c>
     </row>
@@ -3285,7 +3320,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3304,7 +3339,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3313,7 +3348,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3322,7 +3357,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3331,7 +3366,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3340,7 +3375,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3349,7 +3384,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3358,7 +3393,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3367,7 +3402,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3376,8 +3411,8 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <f>Data!$I$26*About!$A$28</f>
-        <v>20.282351007638955</v>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A10,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
+        <v>17.683353636823785</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3385,7 +3420,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3394,7 +3429,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3403,7 +3438,7 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3412,7 +3447,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3421,7 +3456,7 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3430,7 +3465,7 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3439,7 +3474,7 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3448,7 +3483,7 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3457,7 +3492,7 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3466,7 +3501,7 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3475,7 +3510,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3484,7 +3519,7 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3493,7 +3528,7 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3502,7 +3537,7 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3511,7 +3546,7 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3520,7 +3555,7 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3537,7 +3572,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3556,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A2,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3565,7 +3600,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A3,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3574,7 +3609,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A4,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3583,7 +3618,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A5,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3592,7 +3627,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A6,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3601,7 +3636,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A7,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3610,7 +3645,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A8,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3619,7 +3654,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A9,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3628,7 +3663,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>Data!$I$27*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3637,8 +3672,8 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <f>Data!$I$26*About!$A$28</f>
-        <v>20.282351007638955</v>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A11,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
+        <v>5.6086039039939504</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3646,7 +3681,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A12,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3655,7 +3690,7 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A13,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3664,8 +3699,8 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <f>Data!$I$26*About!$A$28</f>
-        <v>20.282351007638955</v>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A14,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
+        <v>14.98211642730281</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3673,8 +3708,8 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <f>Data!$I$26*About!$A$28</f>
-        <v>20.282351007638955</v>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A15,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
+        <v>7.8803717282670158</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3682,7 +3717,7 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A16,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3691,7 +3726,7 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A17,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3700,7 +3735,7 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A18,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3709,7 +3744,7 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A19,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3718,7 +3753,7 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A20,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3727,7 +3762,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A21,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3736,7 +3771,7 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A22,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3745,7 +3780,7 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A23,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3754,8 +3789,8 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <f>Data!$I$26*About!$A$28</f>
-        <v>20.282351007638955</v>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A24,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
+        <v>5.1296563722232209</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -3763,7 +3798,7 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A25,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3772,7 +3807,7 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <f>Data!$I$26*About!$A$28</f>
+        <f>IFERROR(INDEX(Data!$27:$27,MATCH('CC-CCoIPCE'!A26,Data!$22:$22,0)),Data!$I$27)*About!$A$28</f>
         <v>20.282351007638955</v>
       </c>
     </row>
@@ -3808,7 +3843,7 @@
         <v>79</v>
       </c>
       <c r="B2">
-        <f>Data!E26*About!$A$28</f>
+        <f>Data!E27*About!$A$28</f>
         <v>10.538813788488513</v>
       </c>
     </row>
@@ -3824,8 +3859,8 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3875,14 +3910,14 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E2">
@@ -3912,14 +3947,14 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E3">
@@ -3949,14 +3984,14 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E4">
@@ -3986,14 +4021,14 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E5">
@@ -4023,14 +4058,14 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E6">
@@ -4060,14 +4095,14 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E7">
@@ -4097,14 +4132,14 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E8">
@@ -4134,14 +4169,14 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E9">
@@ -4171,15 +4206,15 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <f>Data!$I$24/10^12</f>
-        <v>5.4594256000000005E-7</v>
+        <f>IFERROR(INDEX(Data!$25:$25,MATCH('CC-CCoIPCE'!A10,Data!$22:$22,0)),Data!$I$25)*About!$A$28/10^12</f>
+        <v>4.2377253712384721E-7</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <f>Data!$I$25/10^12</f>
-        <v>8.8715665999999999E-6</v>
+        <f>IFERROR(INDEX(Data!$26:$26,MATCH('CC-CCoIPCE'!A10,Data!$22:$22,0)),Data!$I$26)*About!$A$28/10^12</f>
+        <v>7.7187140690415008E-6</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4208,14 +4243,14 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E11">
@@ -4245,14 +4280,14 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E12">
@@ -4282,14 +4317,14 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E13">
@@ -4319,14 +4354,14 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E14">
@@ -4356,14 +4391,14 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E15">
@@ -4393,14 +4428,14 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E16">
@@ -4430,14 +4465,14 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E17">
@@ -4467,14 +4502,14 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E18">
@@ -4504,14 +4539,14 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E19">
@@ -4541,14 +4576,14 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E20">
@@ -4578,14 +4613,14 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E21">
@@ -4615,14 +4650,14 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E22">
@@ -4652,14 +4687,14 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E23">
@@ -4689,14 +4724,14 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E24">
@@ -4726,14 +4761,14 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E25">
@@ -4763,14 +4798,14 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <f>Data!$I$24/10^12</f>
+        <f>Data!$I$25/10^12</f>
         <v>5.4594256000000005E-7</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <f>Data!$I$25/10^12</f>
+        <f>Data!$I$26/10^12</f>
         <v>8.8715665999999999E-6</v>
       </c>
       <c r="E26">

</xml_diff>

<commit_message>
Adds green/low carbon hydrogen if subscript elements, feeds demand through new structure
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC8057-3D10-459B-A73B-36B6485E5AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8FFF93-ACC1-4A89-AA71-AD1CFE45439B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60840" yWindow="2385" windowWidth="24900" windowHeight="14490" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="102">
   <si>
     <t>Source:</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>hydrogen electrolysis in our BAU case.</t>
+  </si>
+  <si>
+    <t>green hydrogen</t>
+  </si>
+  <si>
+    <t>low carbon hydrogen</t>
+  </si>
+  <si>
+    <t>green hydrogen if</t>
+  </si>
+  <si>
+    <t>low carbon hydrogen if</t>
   </si>
 </sst>
 </file>
@@ -750,7 +762,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -904,10 +916,10 @@
   <sheetPr codeName="Sheet11">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +929,7 @@
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
@@ -951,8 +963,14 @@
       <c r="K1" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -988,8 +1006,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1025,8 +1049,14 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1062,8 +1092,14 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1099,8 +1135,14 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1136,8 +1178,14 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1173,8 +1221,14 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1210,8 +1264,14 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1247,8 +1307,14 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1285,8 +1351,14 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1322,8 +1394,14 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1359,8 +1437,14 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1396,8 +1480,14 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1433,8 +1523,14 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1470,8 +1566,14 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1507,8 +1609,14 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1544,8 +1652,14 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1581,8 +1695,14 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1618,8 +1738,14 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1655,8 +1781,14 @@
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1692,8 +1824,14 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1729,8 +1867,14 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1766,8 +1910,14 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1803,8 +1953,14 @@
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1840,8 +1996,14 @@
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1875,6 +2037,12 @@
         <v>0</v>
       </c>
       <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>0</v>
       </c>
     </row>
@@ -1888,10 +2056,10 @@
   <sheetPr codeName="Sheet13">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1993,6 +2161,22 @@
         <v>94</v>
       </c>
       <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
         <v>0</v>
       </c>
     </row>
@@ -2960,7 +3144,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3857,10 +4041,10 @@
   <sheetPr codeName="Sheet10">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3870,7 +4054,7 @@
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
@@ -3904,8 +4088,14 @@
       <c r="K1" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3941,8 +4131,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3978,8 +4174,14 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4015,8 +4217,14 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4052,8 +4260,14 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -4089,8 +4303,14 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4126,8 +4346,14 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -4163,8 +4389,14 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4200,8 +4432,14 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4237,8 +4475,14 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4274,8 +4518,14 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -4311,8 +4561,14 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4348,8 +4604,14 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4385,8 +4647,14 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4422,8 +4690,14 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4459,8 +4733,14 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4496,8 +4776,14 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4533,8 +4819,14 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4570,8 +4862,14 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -4607,8 +4905,14 @@
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -4644,8 +4948,14 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -4681,8 +4991,14 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -4718,8 +5034,14 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -4755,8 +5077,14 @@
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -4792,8 +5120,14 @@
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -4827,6 +5161,12 @@
         <v>0</v>
       </c>
       <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>0</v>
       </c>
     </row>

</xml_diff>